<commit_message>
Add charging infrastructure costs
</commit_message>
<xml_diff>
--- a/dev/Input data_truck.xlsx
+++ b/dev/Input data_truck.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/carculator_truck/dev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E488256-D938-CB4D-AA40-0BF011A692CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B831B8C-FBC7-2C46-A282-712E2E13E806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1480" yWindow="760" windowWidth="28760" windowHeight="18880" tabRatio="518" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1620,10 +1620,10 @@
   <dimension ref="A1:AU387"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="11" ySplit="2" topLeftCell="X48" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="11" ySplit="2" topLeftCell="L133" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AA53" sqref="AA53:AC53"/>
+      <selection pane="bottomRight" activeCell="E133" sqref="E133:L334"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -4188,7 +4188,7 @@
         <v>5350.0199999999995</v>
       </c>
     </row>
-    <row r="27" spans="1:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>56</v>
       </c>
@@ -4277,7 +4277,7 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>56</v>
       </c>
@@ -4358,7 +4358,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>56</v>
       </c>
@@ -4439,7 +4439,7 @@
         <v>900</v>
       </c>
     </row>
-    <row r="30" spans="1:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>56</v>
       </c>
@@ -4528,7 +4528,7 @@
         <v>3235.2</v>
       </c>
     </row>
-    <row r="31" spans="1:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>56</v>
       </c>
@@ -4617,7 +4617,7 @@
         <v>3235.2</v>
       </c>
     </row>
-    <row r="32" spans="1:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>56</v>
       </c>
@@ -4706,7 +4706,7 @@
         <v>3806.3999999999996</v>
       </c>
     </row>
-    <row r="33" spans="1:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>56</v>
       </c>
@@ -4795,7 +4795,7 @@
         <v>4393.2</v>
       </c>
     </row>
-    <row r="34" spans="1:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>56</v>
       </c>
@@ -4884,7 +4884,7 @@
         <v>4393.2</v>
       </c>
     </row>
-    <row r="35" spans="1:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>56</v>
       </c>
@@ -4973,7 +4973,7 @@
         <v>4393.2</v>
       </c>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>56</v>
       </c>
@@ -5054,7 +5054,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>56</v>
       </c>
@@ -5135,7 +5135,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>56</v>
       </c>
@@ -5216,7 +5216,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="39" spans="1:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>56</v>
       </c>
@@ -5317,7 +5317,7 @@
         <v>18.700000000000003</v>
       </c>
     </row>
-    <row r="40" spans="1:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>56</v>
       </c>
@@ -5418,7 +5418,7 @@
         <v>18.700000000000003</v>
       </c>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>56</v>
       </c>
@@ -5475,7 +5475,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>56</v>
       </c>
@@ -5550,7 +5550,7 @@
         <v>59.876121804653181</v>
       </c>
     </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>56</v>
       </c>
@@ -5625,7 +5625,7 @@
         <v>97.29869793256141</v>
       </c>
     </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>56</v>
       </c>
@@ -5700,7 +5700,7 @@
         <v>82.329667481398118</v>
       </c>
     </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>56</v>
       </c>
@@ -5775,7 +5775,7 @@
         <v>119.75224360930636</v>
       </c>
     </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>56</v>
       </c>
@@ -5850,7 +5850,7 @@
         <v>71.10289464302565</v>
       </c>
     </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>56</v>
       </c>
@@ -5925,7 +5925,7 @@
         <v>89.814182706979764</v>
       </c>
     </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>56</v>
       </c>
@@ -6000,7 +6000,7 @@
         <v>86.071925094188941</v>
       </c>
     </row>
-    <row r="49" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>56</v>
       </c>
@@ -6075,7 +6075,7 @@
         <v>82.329667481398118</v>
       </c>
     </row>
-    <row r="50" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>56</v>
       </c>
@@ -6150,7 +6150,7 @@
         <v>74.845152255816473</v>
       </c>
     </row>
-    <row r="51" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>56</v>
       </c>
@@ -6225,7 +6225,7 @@
         <v>67.360637030234827</v>
       </c>
     </row>
-    <row r="52" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>56</v>
       </c>
@@ -6300,7 +6300,7 @@
         <v>74.845152255816473</v>
       </c>
     </row>
-    <row r="53" spans="1:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>56</v>
       </c>
@@ -6387,7 +6387,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="54" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>56</v>
       </c>
@@ -6494,7 +6494,7 @@
         <v>0.16499999999999998</v>
       </c>
     </row>
-    <row r="55" spans="1:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>56</v>
       </c>
@@ -6597,7 +6597,7 @@
         <v>0.19565217391304351</v>
       </c>
     </row>
-    <row r="56" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>56</v>
       </c>
@@ -6684,7 +6684,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="57" spans="1:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>56</v>
       </c>
@@ -6785,7 +6785,7 @@
         <v>253.00000000000003</v>
       </c>
     </row>
-    <row r="58" spans="1:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>56</v>
       </c>
@@ -6884,7 +6884,7 @@
         <v>715.00000000000011</v>
       </c>
     </row>
-    <row r="59" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>56</v>
       </c>
@@ -6965,7 +6965,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="60" spans="1:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>56</v>
       </c>
@@ -7064,7 +7064,7 @@
         <v>68.2</v>
       </c>
     </row>
-    <row r="61" spans="1:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>56</v>
       </c>
@@ -7149,7 +7149,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="62" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>56</v>
       </c>
@@ -7230,7 +7230,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="63" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>56</v>
       </c>
@@ -7331,7 +7331,7 @@
         <v>2.5850000000000001E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>56</v>
       </c>
@@ -7432,7 +7432,7 @@
         <v>2.5850000000000001E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>56</v>
       </c>
@@ -7533,7 +7533,7 @@
         <v>2.5850000000000001E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>56</v>
       </c>
@@ -7634,7 +7634,7 @@
         <v>2.5850000000000001E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>56</v>
       </c>
@@ -7735,7 +7735,7 @@
         <v>2.5850000000000001E-2</v>
       </c>
     </row>
-    <row r="68" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>56</v>
       </c>
@@ -7836,7 +7836,7 @@
         <v>2.5850000000000001E-2</v>
       </c>
     </row>
-    <row r="69" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>56</v>
       </c>
@@ -8026,7 +8026,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="71" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>56</v>
       </c>
@@ -8127,7 +8127,7 @@
         <v>8.2500000000000004E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>56</v>
       </c>
@@ -8228,7 +8228,7 @@
         <v>8.2500000000000004E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>56</v>
       </c>
@@ -8329,7 +8329,7 @@
         <v>0.11561</v>
       </c>
     </row>
-    <row r="74" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>56</v>
       </c>
@@ -8430,7 +8430,7 @@
         <v>0.14563999999999999</v>
       </c>
     </row>
-    <row r="75" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>56</v>
       </c>
@@ -8531,7 +8531,7 @@
         <v>0.14563999999999999</v>
       </c>
     </row>
-    <row r="76" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>56</v>
       </c>
@@ -8632,7 +8632,7 @@
         <v>0.14563999999999999</v>
       </c>
     </row>
-    <row r="77" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
         <v>56</v>
       </c>
@@ -8733,7 +8733,7 @@
         <v>0.14563999999999999</v>
       </c>
     </row>
-    <row r="78" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>56</v>
       </c>
@@ -8834,7 +8834,7 @@
         <v>0.12100000000000001</v>
       </c>
     </row>
-    <row r="79" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>56</v>
       </c>
@@ -8935,7 +8935,7 @@
         <v>0.17347000000000001</v>
       </c>
     </row>
-    <row r="80" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
         <v>56</v>
       </c>
@@ -9036,7 +9036,7 @@
         <v>0.20350000000000001</v>
       </c>
     </row>
-    <row r="81" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>56</v>
       </c>
@@ -9137,7 +9137,7 @@
         <v>0.20350000000000001</v>
       </c>
     </row>
-    <row r="82" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
         <v>56</v>
       </c>
@@ -9238,7 +9238,7 @@
         <v>0.20350000000000001</v>
       </c>
     </row>
-    <row r="83" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>56</v>
       </c>
@@ -9339,7 +9339,7 @@
         <v>0.20350000000000001</v>
       </c>
     </row>
-    <row r="84" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
         <v>56</v>
       </c>
@@ -9440,7 +9440,7 @@
         <v>0.20350000000000001</v>
       </c>
     </row>
-    <row r="85" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>56</v>
       </c>
@@ -9541,7 +9541,7 @@
         <v>0.12100000000000001</v>
       </c>
     </row>
-    <row r="86" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
         <v>56</v>
       </c>
@@ -9642,7 +9642,7 @@
         <v>0.12100000000000001</v>
       </c>
     </row>
-    <row r="87" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>56</v>
       </c>
@@ -9743,7 +9743,7 @@
         <v>0.17347000000000001</v>
       </c>
     </row>
-    <row r="88" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
         <v>56</v>
       </c>
@@ -9844,7 +9844,7 @@
         <v>0.17347000000000001</v>
       </c>
     </row>
-    <row r="89" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
         <v>56</v>
       </c>
@@ -9945,7 +9945,7 @@
         <v>0.20350000000000001</v>
       </c>
     </row>
-    <row r="90" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
         <v>56</v>
       </c>
@@ -10046,7 +10046,7 @@
         <v>0.20350000000000001</v>
       </c>
     </row>
-    <row r="91" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
         <v>56</v>
       </c>
@@ -10714,7 +10714,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="99" spans="1:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
         <v>56</v>
       </c>
@@ -10801,7 +10801,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="100" spans="1:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
         <v>56</v>
       </c>
@@ -10902,7 +10902,7 @@
         <v>1.1000000000000001E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
         <v>56</v>
       </c>
@@ -11003,7 +11003,7 @@
         <v>3.6300000000000006E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
         <v>56</v>
       </c>
@@ -11104,7 +11104,7 @@
         <v>0.10340000000000001</v>
       </c>
     </row>
-    <row r="103" spans="1:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>56</v>
       </c>
@@ -11205,7 +11205,7 @@
         <v>0.1716</v>
       </c>
     </row>
-    <row r="104" spans="1:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
         <v>56</v>
       </c>
@@ -11306,7 +11306,7 @@
         <v>0.1716</v>
       </c>
     </row>
-    <row r="105" spans="1:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
         <v>56</v>
       </c>
@@ -11407,7 +11407,7 @@
         <v>0.1716</v>
       </c>
     </row>
-    <row r="106" spans="1:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
         <v>56</v>
       </c>
@@ -11508,7 +11508,7 @@
         <v>0.1716</v>
       </c>
     </row>
-    <row r="107" spans="1:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
         <v>56</v>
       </c>
@@ -11609,7 +11609,7 @@
         <v>5.5000000000000005E-3</v>
       </c>
     </row>
-    <row r="108" spans="1:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
         <v>56</v>
       </c>
@@ -11710,7 +11710,7 @@
         <v>1.8700000000000001E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
         <v>56</v>
       </c>
@@ -11811,7 +11811,7 @@
         <v>5.1700000000000003E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
         <v>56</v>
       </c>
@@ -11912,7 +11912,7 @@
         <v>8.5800000000000001E-2</v>
       </c>
     </row>
-    <row r="111" spans="1:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
         <v>56</v>
       </c>
@@ -12013,7 +12013,7 @@
         <v>8.5800000000000001E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
         <v>56</v>
       </c>
@@ -13890,7 +13890,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A133" s="3" t="s">
         <v>29</v>
       </c>
@@ -13981,7 +13981,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="134" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A134" s="3" t="s">
         <v>29</v>
       </c>
@@ -14066,7 +14066,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="135" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A135" s="3" t="s">
         <v>29</v>
       </c>
@@ -14165,7 +14165,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="136" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A136" s="3" t="s">
         <v>29</v>
       </c>
@@ -32111,7 +32111,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="327" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A327" s="3" t="s">
         <v>29</v>
       </c>
@@ -32210,7 +32210,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="328" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A328" s="3" t="s">
         <v>29</v>
       </c>
@@ -32309,7 +32309,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="329" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A329" s="3" t="s">
         <v>29</v>
       </c>
@@ -32408,7 +32408,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="330" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A330" s="3" t="s">
         <v>29</v>
       </c>
@@ -32507,7 +32507,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="331" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A331" s="3" t="s">
         <v>29</v>
       </c>
@@ -32606,7 +32606,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="332" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A332" s="3" t="s">
         <v>29</v>
       </c>
@@ -32697,7 +32697,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="333" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A333" s="3" t="s">
         <v>29</v>
       </c>
@@ -32799,7 +32799,7 @@
         <v>11646.250000000004</v>
       </c>
     </row>
-    <row r="334" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A334" s="3" t="s">
         <v>29</v>
       </c>
@@ -32901,7 +32901,7 @@
         <v>11646.250000000004</v>
       </c>
     </row>
-    <row r="335" spans="1:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A335" s="3" t="s">
         <v>56</v>
       </c>
@@ -33002,7 +33002,7 @@
         <v>8.5800000000000001E-2</v>
       </c>
     </row>
-    <row r="336" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:29" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
       <c r="A336" s="3" t="s">
         <v>56</v>
       </c>
@@ -33439,7 +33439,7 @@
         <v>4.0000000000000003E-5</v>
       </c>
     </row>
-    <row r="341" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A341" s="3" t="s">
         <v>56</v>
       </c>
@@ -35239,7 +35239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="366" spans="1:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A366" s="3" t="s">
         <v>56</v>
       </c>
@@ -35326,7 +35326,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="367" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A367" s="3" t="s">
         <v>56</v>
       </c>
@@ -35433,7 +35433,7 @@
         <v>0.16499999999999998</v>
       </c>
     </row>
-    <row r="368" spans="1:29" ht="15" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:29" ht="15" hidden="1" x14ac:dyDescent="0.2">
       <c r="A368" s="3" t="s">
         <v>56</v>
       </c>
@@ -35538,7 +35538,7 @@
         <v>0.19565217391304351</v>
       </c>
     </row>
-    <row r="369" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A369" s="3" t="s">
         <v>56</v>
       </c>
@@ -36971,34 +36971,18 @@
   <autoFilter ref="A2:AC387" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="4">
       <filters>
-        <filter val="adblue cost per kg"/>
-        <filter val="battery onboard charging infrastructure cost"/>
-        <filter val="combustion exhaust treatment cost"/>
-        <filter val="combustion powertrain cost per kW"/>
-        <filter val="electric powertrain cost per kW"/>
-        <filter val="energy battery cost per kWh, LFP"/>
-        <filter val="energy battery cost per kWh, Li-O2"/>
-        <filter val="energy battery cost per kWh, Li-S"/>
-        <filter val="energy battery cost per kWh, LTO"/>
-        <filter val="energy battery cost per kWh, NCA"/>
-        <filter val="energy battery cost per kWh, NMC-111"/>
-        <filter val="energy battery cost per kWh, NMC-523"/>
-        <filter val="energy battery cost per kWh, NMC-622"/>
-        <filter val="energy battery cost per kWh, NMC-811"/>
-        <filter val="energy battery cost per kWh, NMC-955"/>
-        <filter val="energy battery cost per kWh, SiB"/>
-        <filter val="energy cost per kWh (depot)"/>
-        <filter val="energy cost per kWh (public)"/>
-        <filter val="fuel cell cost per kW"/>
-        <filter val="fuel tank cost per kg"/>
-        <filter val="glider base cost per kg"/>
-        <filter val="glider lightweighting cost per kg"/>
-        <filter val="heat pump cost"/>
-        <filter val="insurance cost share per year"/>
-        <filter val="insured share of purchase cost"/>
-        <filter val="maintenance cost per km"/>
-        <filter val="power battery cost per kW"/>
-        <filter val="road toll cost per km"/>
+        <filter val="battery cycle life, LFP"/>
+        <filter val="battery cycle life, Li-O2"/>
+        <filter val="battery cycle life, Li-S"/>
+        <filter val="battery cycle life, LTO"/>
+        <filter val="battery cycle life, NCA"/>
+        <filter val="battery cycle life, NMC"/>
+        <filter val="battery cycle life, NMC-111"/>
+        <filter val="battery cycle life, NMC-523"/>
+        <filter val="battery cycle life, NMC-622"/>
+        <filter val="battery cycle life, NMC-811"/>
+        <filter val="battery cycle life, NMC-955"/>
+        <filter val="battery cycle life, SiB"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Improve charger fraction in inventories.
</commit_message>
<xml_diff>
--- a/dev/Input data_truck.xlsx
+++ b/dev/Input data_truck.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10905"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romain/GitHub/carculator_truck/dev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F936384-99AE-F946-8AF6-C8094475D6A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105AE367-78D3-384B-8EB8-222C9EF14A4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4440" yWindow="760" windowWidth="25800" windowHeight="18880" tabRatio="518" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3998" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3998" uniqueCount="347">
   <si>
     <t>power to mass ratio</t>
   </si>
@@ -1091,6 +1091,9 @@
   <si>
     <t>ICEV-d, HEV-d, ICEV-g, FCEV, PHEV-c-d</t>
   </si>
+  <si>
+    <t>€/kW/year</t>
+  </si>
 </sst>
 </file>
 
@@ -1620,10 +1623,10 @@
   <dimension ref="A1:AU387"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="11" ySplit="2" topLeftCell="L71" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="11" ySplit="2" topLeftCell="U301" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B394" sqref="B394"/>
+      <selection pane="bottomRight" activeCell="U378" sqref="U378"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.33203125" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -8026,7 +8029,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="71" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>56</v>
       </c>
@@ -8127,7 +8130,7 @@
         <v>8.2500000000000004E-2</v>
       </c>
     </row>
-    <row r="72" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>56</v>
       </c>
@@ -8228,7 +8231,7 @@
         <v>8.2500000000000004E-2</v>
       </c>
     </row>
-    <row r="73" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>56</v>
       </c>
@@ -8329,7 +8332,7 @@
         <v>0.11561</v>
       </c>
     </row>
-    <row r="74" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>56</v>
       </c>
@@ -8430,7 +8433,7 @@
         <v>0.14563999999999999</v>
       </c>
     </row>
-    <row r="75" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>56</v>
       </c>
@@ -8531,7 +8534,7 @@
         <v>0.14563999999999999</v>
       </c>
     </row>
-    <row r="76" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>56</v>
       </c>
@@ -8632,7 +8635,7 @@
         <v>0.14563999999999999</v>
       </c>
     </row>
-    <row r="77" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
         <v>56</v>
       </c>
@@ -8733,7 +8736,7 @@
         <v>0.14563999999999999</v>
       </c>
     </row>
-    <row r="78" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>56</v>
       </c>
@@ -8834,7 +8837,7 @@
         <v>0.12100000000000001</v>
       </c>
     </row>
-    <row r="79" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>56</v>
       </c>
@@ -8935,7 +8938,7 @@
         <v>0.17347000000000001</v>
       </c>
     </row>
-    <row r="80" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
         <v>56</v>
       </c>
@@ -9036,7 +9039,7 @@
         <v>0.20350000000000001</v>
       </c>
     </row>
-    <row r="81" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>56</v>
       </c>
@@ -9137,7 +9140,7 @@
         <v>0.20350000000000001</v>
       </c>
     </row>
-    <row r="82" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
         <v>56</v>
       </c>
@@ -9238,7 +9241,7 @@
         <v>0.20350000000000001</v>
       </c>
     </row>
-    <row r="83" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>56</v>
       </c>
@@ -9339,7 +9342,7 @@
         <v>0.20350000000000001</v>
       </c>
     </row>
-    <row r="84" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
         <v>56</v>
       </c>
@@ -9440,7 +9443,7 @@
         <v>0.20350000000000001</v>
       </c>
     </row>
-    <row r="85" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>56</v>
       </c>
@@ -9541,7 +9544,7 @@
         <v>0.12100000000000001</v>
       </c>
     </row>
-    <row r="86" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
         <v>56</v>
       </c>
@@ -9642,7 +9645,7 @@
         <v>0.12100000000000001</v>
       </c>
     </row>
-    <row r="87" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>56</v>
       </c>
@@ -9743,7 +9746,7 @@
         <v>0.17347000000000001</v>
       </c>
     </row>
-    <row r="88" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
         <v>56</v>
       </c>
@@ -9844,7 +9847,7 @@
         <v>0.17347000000000001</v>
       </c>
     </row>
-    <row r="89" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
         <v>56</v>
       </c>
@@ -9945,7 +9948,7 @@
         <v>0.20350000000000001</v>
       </c>
     </row>
-    <row r="90" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
         <v>56</v>
       </c>
@@ -10046,7 +10049,7 @@
         <v>0.20350000000000001</v>
       </c>
     </row>
-    <row r="91" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
         <v>56</v>
       </c>
@@ -29829,7 +29832,7 @@
         <v/>
       </c>
     </row>
-    <row r="301" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A301" s="3" t="s">
         <v>27</v>
       </c>
@@ -29995,7 +29998,7 @@
       <c r="AB302" s="5"/>
       <c r="AC302" s="5"/>
     </row>
-    <row r="303" spans="1:31" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:31" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A303" s="3" t="s">
         <v>29</v>
       </c>
@@ -35625,7 +35628,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="370" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A370" s="3" t="s">
         <v>331</v>
       </c>
@@ -35710,7 +35713,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="371" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A371" s="3" t="s">
         <v>331</v>
       </c>
@@ -35795,7 +35798,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="372" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A372" s="3" t="s">
         <v>331</v>
       </c>
@@ -35880,7 +35883,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="373" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A373" s="3" t="s">
         <v>331</v>
       </c>
@@ -35965,7 +35968,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="374" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A374" s="3" t="s">
         <v>331</v>
       </c>
@@ -35982,7 +35985,7 @@
         <v>343</v>
       </c>
       <c r="F374" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G374" s="3" t="s">
         <v>85</v>
@@ -36050,7 +36053,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="375" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A375" s="3" t="s">
         <v>331</v>
       </c>
@@ -36067,7 +36070,7 @@
         <v>336</v>
       </c>
       <c r="F375" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G375" s="3" t="s">
         <v>85</v>
@@ -36081,61 +36084,61 @@
         <v>66</v>
       </c>
       <c r="L375" s="3">
-        <v>80</v>
+        <v>150</v>
       </c>
       <c r="M375" s="3">
-        <v>60</v>
+        <v>100</v>
       </c>
       <c r="N375" s="3">
+        <v>200</v>
+      </c>
+      <c r="O375" s="3">
+        <v>150</v>
+      </c>
+      <c r="P375" s="3">
         <v>100</v>
       </c>
-      <c r="O375" s="3">
-        <v>80</v>
-      </c>
-      <c r="P375" s="3">
-        <v>60</v>
-      </c>
       <c r="Q375" s="3">
+        <v>200</v>
+      </c>
+      <c r="R375" s="3">
+        <v>150</v>
+      </c>
+      <c r="S375" s="3">
         <v>100</v>
       </c>
-      <c r="R375" s="3">
-        <v>80</v>
-      </c>
-      <c r="S375" s="3">
-        <v>60</v>
-      </c>
       <c r="T375" s="3">
+        <v>200</v>
+      </c>
+      <c r="U375" s="3">
+        <v>150</v>
+      </c>
+      <c r="V375" s="3">
         <v>100</v>
       </c>
-      <c r="U375" s="3">
-        <v>80</v>
-      </c>
-      <c r="V375" s="3">
-        <v>60</v>
-      </c>
       <c r="W375" s="3">
+        <v>200</v>
+      </c>
+      <c r="X375" s="3">
+        <v>150</v>
+      </c>
+      <c r="Y375" s="3">
         <v>100</v>
       </c>
-      <c r="X375" s="3">
-        <v>80</v>
-      </c>
-      <c r="Y375" s="3">
-        <v>60</v>
-      </c>
       <c r="Z375" s="3">
+        <v>200</v>
+      </c>
+      <c r="AA375" s="3">
+        <v>150</v>
+      </c>
+      <c r="AB375" s="3">
         <v>100</v>
       </c>
-      <c r="AA375" s="3">
-        <v>80</v>
-      </c>
-      <c r="AB375" s="3">
-        <v>60</v>
-      </c>
       <c r="AC375" s="3">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="376" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="376" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A376" s="3" t="s">
         <v>331</v>
       </c>
@@ -36152,7 +36155,7 @@
         <v>337</v>
       </c>
       <c r="F376" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G376" s="3" t="s">
         <v>85</v>
@@ -36166,61 +36169,61 @@
         <v>66</v>
       </c>
       <c r="L376" s="3">
-        <v>170</v>
+        <v>200</v>
       </c>
       <c r="M376" s="3">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="N376" s="3">
+        <v>400</v>
+      </c>
+      <c r="O376" s="3">
         <v>200</v>
       </c>
-      <c r="O376" s="3">
-        <v>170</v>
-      </c>
       <c r="P376" s="3">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="Q376" s="3">
+        <v>400</v>
+      </c>
+      <c r="R376" s="3">
         <v>200</v>
       </c>
-      <c r="R376" s="3">
-        <v>170</v>
-      </c>
       <c r="S376" s="3">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="T376" s="3">
+        <v>400</v>
+      </c>
+      <c r="U376" s="3">
         <v>200</v>
       </c>
-      <c r="U376" s="3">
-        <v>170</v>
-      </c>
       <c r="V376" s="3">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="W376" s="3">
+        <v>400</v>
+      </c>
+      <c r="X376" s="3">
         <v>200</v>
       </c>
-      <c r="X376" s="3">
-        <v>170</v>
-      </c>
       <c r="Y376" s="3">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="Z376" s="3">
+        <v>400</v>
+      </c>
+      <c r="AA376" s="3">
         <v>200</v>
       </c>
-      <c r="AA376" s="3">
-        <v>170</v>
-      </c>
       <c r="AB376" s="3">
-        <v>150</v>
+        <v>0</v>
       </c>
       <c r="AC376" s="3">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="377" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="377" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A377" s="3" t="s">
         <v>331</v>
       </c>
@@ -36307,7 +36310,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="378" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A378" s="3" t="s">
         <v>331</v>
       </c>
@@ -36324,7 +36327,7 @@
         <v>341</v>
       </c>
       <c r="F378" s="3" t="s">
-        <v>98</v>
+        <v>346</v>
       </c>
       <c r="G378" s="3" t="s">
         <v>85</v>
@@ -36340,61 +36343,61 @@
         <v>66</v>
       </c>
       <c r="L378" s="3">
-        <v>40</v>
+        <v>140</v>
       </c>
       <c r="M378" s="3">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="N378" s="3">
-        <v>60</v>
+        <v>180</v>
       </c>
       <c r="O378" s="3">
-        <v>40</v>
+        <v>140</v>
       </c>
       <c r="P378" s="3">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="Q378" s="3">
-        <v>60</v>
+        <v>180</v>
       </c>
       <c r="R378" s="3">
-        <v>40</v>
+        <v>140</v>
       </c>
       <c r="S378" s="3">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="T378" s="3">
-        <v>60</v>
+        <v>180</v>
       </c>
       <c r="U378" s="3">
-        <v>40</v>
+        <v>140</v>
       </c>
       <c r="V378" s="3">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="W378" s="3">
-        <v>60</v>
+        <v>180</v>
       </c>
       <c r="X378" s="3">
-        <v>40</v>
+        <v>140</v>
       </c>
       <c r="Y378" s="3">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="Z378" s="3">
-        <v>60</v>
+        <v>180</v>
       </c>
       <c r="AA378" s="3">
-        <v>40</v>
+        <v>140</v>
       </c>
       <c r="AB378" s="3">
-        <v>20</v>
+        <v>100</v>
       </c>
       <c r="AC378" s="3">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="379" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="379" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A379" s="3" t="s">
         <v>331</v>
       </c>
@@ -36479,7 +36482,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="380" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A380" s="3" t="s">
         <v>331</v>
       </c>
@@ -36540,7 +36543,7 @@
       <c r="AB380" s="3"/>
       <c r="AC380" s="3"/>
     </row>
-    <row r="381" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A381" s="3" t="s">
         <v>331</v>
       </c>
@@ -36601,7 +36604,7 @@
       <c r="AB381" s="3"/>
       <c r="AC381" s="3"/>
     </row>
-    <row r="382" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A382" s="3" t="s">
         <v>331</v>
       </c>
@@ -36662,7 +36665,7 @@
       <c r="AB382" s="3"/>
       <c r="AC382" s="3"/>
     </row>
-    <row r="383" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A383" s="3" t="s">
         <v>331</v>
       </c>
@@ -36723,7 +36726,7 @@
       <c r="AB383" s="3"/>
       <c r="AC383" s="3"/>
     </row>
-    <row r="384" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A384" s="3" t="s">
         <v>331</v>
       </c>
@@ -36784,7 +36787,7 @@
       <c r="AB384" s="3"/>
       <c r="AC384" s="3"/>
     </row>
-    <row r="385" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A385" s="3" t="s">
         <v>331</v>
       </c>
@@ -36845,7 +36848,7 @@
       <c r="AB385" s="3"/>
       <c r="AC385" s="3"/>
     </row>
-    <row r="386" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A386" s="3" t="s">
         <v>331</v>
       </c>
@@ -36906,7 +36909,7 @@
       <c r="AB386" s="3"/>
       <c r="AC386" s="3"/>
     </row>
-    <row r="387" spans="1:29" hidden="1" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A387" s="3" t="s">
         <v>331</v>
       </c>
@@ -36971,7 +36974,16 @@
   <autoFilter ref="A2:AC387" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <filterColumn colId="4">
       <filters>
-        <filter val="maintenance cost per km"/>
+        <filter val="charger efficiency"/>
+        <filter val="charger mass"/>
+        <filter val="depot charger capacity charger per kW-year"/>
+        <filter val="depot charger capex per kW"/>
+        <filter val="depot charger connection per kW"/>
+        <filter val="depot charger installation per kW"/>
+        <filter val="depot charger lifetime"/>
+        <filter val="depot charger O&amp;M share"/>
+        <filter val="depot charger power"/>
+        <filter val="trucks per depot charger"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>